<commit_message>
Not sure what these changes are.  They're quite old.  But I'm committing them anyway.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -125,7 +125,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,14 +141,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -156,6 +163,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -163,6 +173,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -503,7 +516,7 @@
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -538,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -556,7 +569,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -573,8 +586,12 @@
         <f>ROUND(D$2/D4, 2-INT(LOG(D$2/D4)))</f>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" s="4">
+        <f>E9/E4</f>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -591,8 +608,12 @@
         <f>ROUND(D$2/D5, 2-INT(LOG(D$2/D5)))</f>
         <v>1.61</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5">
+        <f>E14/E4</f>
+        <v>86.875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -610,7 +631,7 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -628,7 +649,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -646,43 +667,43 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2">
-        <v>5104895</v>
+        <v>5184815</v>
       </c>
       <c r="E9" s="3">
         <f>ROUND(D$2/D9, 2-INT(LOG(D$2/D9)))</f>
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2">
-        <v>2005988</v>
+        <v>5104895</v>
       </c>
       <c r="E10" s="3">
         <f>ROUND(D$2/D10, 2-INT(LOG(D$2/D10)))</f>
-        <v>50.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -690,35 +711,35 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2">
-        <v>1932271</v>
+        <v>2005988</v>
       </c>
       <c r="E11" s="3">
         <f>ROUND(D$2/D11, 2-INT(LOG(D$2/D11)))</f>
-        <v>52.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>50.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2">
-        <v>1006979</v>
+        <v>1932271</v>
       </c>
       <c r="E12" s="3">
         <f>ROUND(D$2/D12, 2-INT(LOG(D$2/D12)))</f>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>52.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -729,34 +750,34 @@
         <v>7</v>
       </c>
       <c r="D13" s="2">
-        <v>158887</v>
+        <v>734126</v>
       </c>
       <c r="E13" s="3">
         <f>ROUND(D$2/D13, 2-INT(LOG(D$2/D13)))</f>
-        <v>639</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="2">
-        <v>86872</v>
+        <v>729270</v>
       </c>
       <c r="E14" s="3">
         <f>ROUND(D$2/D14, 2-INT(LOG(D$2/D14)))</f>
-        <v>1170</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:E14">
-    <sortCondition descending="1" ref="D2"/>
+    <sortCondition descending="1" ref="D2:D14"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update summary.xlsx with Atom results
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Language</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Variant</t>
   </si>
   <si>
-    <t>gcc 4.2</t>
-  </si>
-  <si>
     <t>SSE</t>
   </si>
   <si>
@@ -45,31 +42,43 @@
     <t>scalar</t>
   </si>
   <si>
-    <t>clang 2.9</t>
-  </si>
-  <si>
     <t>JavaScript</t>
   </si>
   <si>
-    <t>Chrome 15</t>
-  </si>
-  <si>
     <t>untyped</t>
   </si>
   <si>
     <t>typed arrays</t>
   </si>
   <si>
-    <t>Firefox 7</t>
-  </si>
-  <si>
-    <t>Firefox 9a2</t>
-  </si>
-  <si>
     <t>Emscripten</t>
   </si>
   <si>
     <t>Slowdown</t>
+  </si>
+  <si>
+    <t>Intel Atom D2700</t>
+  </si>
+  <si>
+    <t>Ubuntu 12.04</t>
+  </si>
+  <si>
+    <t>clang 3.1 -O3</t>
+  </si>
+  <si>
+    <t>gcc 4.6.3 -O3</t>
+  </si>
+  <si>
+    <t>node 0.8.14, emscripten -O1</t>
+  </si>
+  <si>
+    <t>Firefox 17</t>
+  </si>
+  <si>
+    <t>Chromium 20.0</t>
+  </si>
+  <si>
+    <t>FASTEST:</t>
   </si>
 </sst>
 </file>
@@ -505,18 +514,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,257 +537,231 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2">
+        <f>MAX(D2:D12)</f>
+        <v>24040000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
-        <v>101580000</v>
+        <v>24040000</v>
       </c>
       <c r="E2" s="3">
-        <f>ROUND(D$2/D2, 2-INT(LOG(D$2/D2)))</f>
+        <f>ROUND($H$1/D2, 2-INT(LOG($H$1/D2)))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" s="2">
-        <v>96420454</v>
+        <v>22530000</v>
       </c>
       <c r="E3" s="3">
-        <f>ROUND(D$2/D3, 2-INT(LOG(D$2/D3)))</f>
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>ROUND($H$1/D3, 2-INT(LOG($H$1/D3)))</f>
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>63355501</v>
+        <v>18730000</v>
       </c>
       <c r="E4" s="3">
-        <f>ROUND(D$2/D4, 2-INT(LOG(D$2/D4)))</f>
-        <v>1.6</v>
-      </c>
-      <c r="G4" s="4">
-        <f>E9/E4</f>
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>ROUND($H$1/D4, 2-INT(LOG($H$1/D4)))</f>
+        <v>1.28</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13040000</v>
+      </c>
+      <c r="E5" s="3">
+        <f>ROUND($H$1/D5, 2-INT(LOG($H$1/D5)))</f>
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" s="2">
+        <v>3150000</v>
+      </c>
+      <c r="E6" s="3">
+        <f>ROUND($H$1/D6, 2-INT(LOG($H$1/D6)))</f>
+        <v>7.63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2">
-        <v>62928175</v>
-      </c>
-      <c r="E5" s="3">
-        <f>ROUND(D$2/D5, 2-INT(LOG(D$2/D5)))</f>
-        <v>1.61</v>
-      </c>
-      <c r="G5">
-        <f>E14/E4</f>
-        <v>86.875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D7" s="2">
+        <v>2437562</v>
+      </c>
+      <c r="E7" s="3">
+        <f>ROUND($H$1/D7, 2-INT(LOG($H$1/D7)))</f>
+        <v>9.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1084577</v>
+      </c>
+      <c r="E8" s="3">
+        <f>ROUND($H$1/D8, 2-INT(LOG($H$1/D8)))</f>
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2">
-        <v>10210000</v>
-      </c>
-      <c r="E6" s="3">
-        <f>ROUND(D$2/D6, 2-INT(LOG(D$2/D6)))</f>
-        <v>9.9499999999999993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>944333</v>
+      </c>
+      <c r="E9" s="3">
+        <f>ROUND($H$1/D9, 2-INT(LOG($H$1/D9)))</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D10" s="2">
+        <v>807577</v>
+      </c>
+      <c r="E10" s="3">
+        <f>ROUND($H$1/D10, 2-INT(LOG($H$1/D10)))</f>
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>679802</v>
+      </c>
+      <c r="E11" s="3">
+        <f>ROUND($H$1/D11, 2-INT(LOG($H$1/D11)))</f>
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>677966</v>
+      </c>
+      <c r="E12" s="3">
+        <f>ROUND($H$1/D12, 2-INT(LOG($H$1/D12)))</f>
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2">
-        <v>8401598</v>
-      </c>
-      <c r="E7" s="3">
-        <f>ROUND(D$2/D7, 2-INT(LOG(D$2/D7)))</f>
-        <v>12.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5790000</v>
-      </c>
-      <c r="E8" s="3">
-        <f>ROUND(D$2/D8, 2-INT(LOG(D$2/D8)))</f>
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5184815</v>
-      </c>
-      <c r="E9" s="3">
-        <f>ROUND(D$2/D9, 2-INT(LOG(D$2/D9)))</f>
-        <v>19.600000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5104895</v>
-      </c>
-      <c r="E10" s="3">
-        <f>ROUND(D$2/D10, 2-INT(LOG(D$2/D10)))</f>
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2005988</v>
-      </c>
-      <c r="E11" s="3">
-        <f>ROUND(D$2/D11, 2-INT(LOG(D$2/D11)))</f>
-        <v>50.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1932271</v>
-      </c>
-      <c r="E12" s="3">
-        <f>ROUND(D$2/D12, 2-INT(LOG(D$2/D12)))</f>
-        <v>52.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2">
-        <v>734126</v>
-      </c>
-      <c r="E13" s="3">
-        <f>ROUND(D$2/D13, 2-INT(LOG(D$2/D13)))</f>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2">
-        <v>729270</v>
-      </c>
-      <c r="E14" s="3">
-        <f>ROUND(D$2/D14, 2-INT(LOG(D$2/D14)))</f>
-        <v>139</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E14">
-    <sortCondition descending="1" ref="D2:D14"/>
+  <sortState ref="A2:E12">
+    <sortCondition descending="1" ref="D2:D12"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>